<commit_message>
Added footprints to all components except the connectors and buck-boost converter
</commit_message>
<xml_diff>
--- a/Passives_BOM.xlsx
+++ b/Passives_BOM.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ghani\Documents\ECE Projects\Variable_Voltage_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74A87AE-4C97-437B-A482-07098FFBE085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC1D49-9B3C-4333-8145-899FDEAC061E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5910" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{16F76EAB-28E7-44E5-8787-201DB1EE94CE}"/>
+    <workbookView xWindow="43095" yWindow="-5790" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{16F76EAB-28E7-44E5-8787-201DB1EE94CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors" sheetId="1" r:id="rId1"/>
     <sheet name="Inductor" sheetId="2" r:id="rId2"/>
+    <sheet name="Resistors" sheetId="3" r:id="rId3"/>
+    <sheet name="Potentiometer" sheetId="4" r:id="rId4"/>
+    <sheet name="Switch" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
   <si>
     <t>Capacitance (uF)</t>
   </si>
@@ -178,6 +181,165 @@
   </si>
   <si>
     <t>Saturation Current (A)</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>100kohm</t>
+  </si>
+  <si>
+    <t>RC0402FR-07100KL</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>62.5mW</t>
+  </si>
+  <si>
+    <t>R102, R103</t>
+  </si>
+  <si>
+    <t>RTT025002FTH</t>
+  </si>
+  <si>
+    <t>50kohm</t>
+  </si>
+  <si>
+    <t>11mohm</t>
+  </si>
+  <si>
+    <t>1210W2F110MT5E</t>
+  </si>
+  <si>
+    <t>500mW</t>
+  </si>
+  <si>
+    <t>1210</t>
+  </si>
+  <si>
+    <t>5kohm</t>
+  </si>
+  <si>
+    <t>RT0603BRE075KL</t>
+  </si>
+  <si>
+    <t>100mW</t>
+  </si>
+  <si>
+    <t>4.3kohm</t>
+  </si>
+  <si>
+    <t>RT0805BRD074K3L</t>
+  </si>
+  <si>
+    <t>125mW</t>
+  </si>
+  <si>
+    <t>R111</t>
+  </si>
+  <si>
+    <t>R112</t>
+  </si>
+  <si>
+    <t>160ohm</t>
+  </si>
+  <si>
+    <t>ERJ2RKF1600X</t>
+  </si>
+  <si>
+    <t>R113</t>
+  </si>
+  <si>
+    <t>140kohm</t>
+  </si>
+  <si>
+    <t>RC0603FR-07140KL</t>
+  </si>
+  <si>
+    <t>R117</t>
+  </si>
+  <si>
+    <t>6.4kohm</t>
+  </si>
+  <si>
+    <t>ARG03DTC6401N</t>
+  </si>
+  <si>
+    <t>R114</t>
+  </si>
+  <si>
+    <t>R101, R104, R105, R107-R110, R115</t>
+  </si>
+  <si>
+    <t>R106, R116</t>
+  </si>
+  <si>
+    <t>RC0603FR-079K1L</t>
+  </si>
+  <si>
+    <t>9.1kohm</t>
+  </si>
+  <si>
+    <t>R401</t>
+  </si>
+  <si>
+    <t>2.2kohm</t>
+  </si>
+  <si>
+    <t>RC0603FR-072K2L</t>
+  </si>
+  <si>
+    <t>R402</t>
+  </si>
+  <si>
+    <t>24kohm</t>
+  </si>
+  <si>
+    <t>ERJ2RKF2402X</t>
+  </si>
+  <si>
+    <t>R403</t>
+  </si>
+  <si>
+    <t>4.7kohm</t>
+  </si>
+  <si>
+    <t>R404</t>
+  </si>
+  <si>
+    <t>ERJ2RKF4701X</t>
+  </si>
+  <si>
+    <t>1Mohm</t>
+  </si>
+  <si>
+    <t>PTV09A-4025F-A105</t>
+  </si>
+  <si>
+    <t>50mW</t>
+  </si>
+  <si>
+    <t>Through Hole, Snap In</t>
+  </si>
+  <si>
+    <t>Rv101</t>
+  </si>
+  <si>
+    <t>PTS636SK25SMTRLFS</t>
+  </si>
+  <si>
+    <t>6x3.5</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>SW201</t>
   </si>
 </sst>
 </file>
@@ -837,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C861CBD8-654E-4A2D-8AF2-C12E2372250D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,4 +1056,415 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF030805-4871-47F9-84BF-FC910E8CBFE8}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6">
+        <v>0.1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://jlcpcb.com/partdetail/Yageo-RC0402FR07100KL/C60491" xr:uid="{5ACAF9E4-C7C6-41BF-9AF4-96334EC3231E}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://jlcpcb.com/partdetail/Ralec-RTT025002FTH/C166559" xr:uid="{ECE5F1D4-EED0-460A-B2B1-2E8E38851985}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://jlcpcb.com/partdetail/415373-1210W2F110MT5E/C422423" xr:uid="{6FA550F9-0DFD-44DC-A996-907D52497E4A}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://jlcpcb.com/partdetail/Yageo-RT0603BRE075KL/C862232" xr:uid="{F2ACD917-B7C8-4BF6-8CCC-33B79862B112}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://jlcpcb.com/partdetail/Yageo-RT0805BRD074K3L/C728653" xr:uid="{5E3CDED6-A6F9-4ED2-96EF-2FF453A79FC4}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://jlcpcb.com/partdetail/Panasonic-ERJ2RKF1600X/C413068" xr:uid="{EA8C885E-02CE-4F4A-AE74-54CEC6A7824D}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://jlcpcb.com/partdetail/Yageo-RC0603FR07140KL/C185372" xr:uid="{190EBBA4-85EE-4B0E-86BB-32C71341E8BA}"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://jlcpcb.com/partdetail/VikingTech-ARG03DTC6401N/C3014413" xr:uid="{26D23F8B-CCEE-47EC-9E00-F42902777305}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://jlcpcb.com/partdetail/Yageo-RC0603FR079K1L/C114639" xr:uid="{2C1AC13A-11A2-4ED8-8FF3-ED5E28CFA3FB}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://jlcpcb.com/partdetail/Yageo-RC0603FR072K2L/C114662" xr:uid="{B4CDC09C-A6AB-4B5D-9F10-E21707A2E874}"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://jlcpcb.com/partdetail/Panasonic-ERJ2RKF2402X/C409902" xr:uid="{4635F2C9-B8AD-4301-A283-7CE4A03EF2E5}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://jlcpcb.com/partdetail/Panasonic-ERJ2RKF4701X/C400631" xr:uid="{42BF0948-82BD-46AA-A624-590B69C59AE7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0429A25E-F823-4316-AD90-B6482BD3D0AC}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.digikey.ca/en/products/detail/bourns-inc/PTV09A-4025F-A105/3820576" xr:uid="{B2EFF1C5-BCFC-4CA9-B573-7E48DFCB85FE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82411D3-4A8F-47FA-B40A-869B4356D2FF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://jlcpcb.com/partdetail/ck-PTS636SK25SMTRLFS/C2689642" xr:uid="{6A3B90E7-0893-40E0-8495-83E06A7E962C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Assign footprints to all footprints except the buck-boost converter
</commit_message>
<xml_diff>
--- a/Passives_BOM.xlsx
+++ b/Passives_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ghani\Documents\ECE Projects\Variable_Voltage_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC1D49-9B3C-4333-8145-899FDEAC061E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6282221B-D3CE-42FF-A46B-73B48D1F1F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="-5790" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="4" xr2:uid="{16F76EAB-28E7-44E5-8787-201DB1EE94CE}"/>
+    <workbookView xWindow="43095" yWindow="-5790" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="5" xr2:uid="{16F76EAB-28E7-44E5-8787-201DB1EE94CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Resistors" sheetId="3" r:id="rId3"/>
     <sheet name="Potentiometer" sheetId="4" r:id="rId4"/>
     <sheet name="Switch" sheetId="5" r:id="rId5"/>
+    <sheet name="Connectors" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="124">
   <si>
     <t>Capacitance (uF)</t>
   </si>
@@ -340,6 +341,78 @@
   </si>
   <si>
     <t>SW201</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>Input Voltage Jack</t>
+  </si>
+  <si>
+    <t>PJ-063AH</t>
+  </si>
+  <si>
+    <t>Voltage Rating</t>
+  </si>
+  <si>
+    <t>Current Rating</t>
+  </si>
+  <si>
+    <t>24V</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>5.5mm</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>J101</t>
+  </si>
+  <si>
+    <t>3.5mm</t>
+  </si>
+  <si>
+    <t>Output Voltage Block</t>
+  </si>
+  <si>
+    <t>Input Voltage Block</t>
+  </si>
+  <si>
+    <t>300V</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>J102</t>
+  </si>
+  <si>
+    <t>J103</t>
+  </si>
+  <si>
+    <t>Size (pitch)</t>
+  </si>
+  <si>
+    <t>ST-Link Header</t>
+  </si>
+  <si>
+    <t>PPTC051LFBN-RC</t>
+  </si>
+  <si>
+    <t>250V</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>2.54mm</t>
+  </si>
+  <si>
+    <t>J201</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1440,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,7 +1503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82411D3-4A8F-47FA-B40A-869B4356D2FF}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1467,4 +1540,133 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52525879-3B94-43C6-B780-A84620322222}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1984617</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1984617</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.digikey.ca/en/products/detail/same-sky-formerly-cui-devices/PJ-063AH/2161208" xr:uid="{0CD10D6C-45F9-4247-B9CE-E6D5B9A9BFBD}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.digikey.ca/en/products/detail/phoenix-contact/1984617/950849" xr:uid="{BFF63F18-3D1B-4B36-9C38-162982BB7064}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.digikey.ca/en/products/detail/phoenix-contact/1984617/950849" xr:uid="{519EC28E-AB40-4D6B-B68C-3C7BBCA5A609}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC051LFBN-RC/807239" xr:uid="{85330244-53D4-4E18-8205-702EB6A123B4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Routed signal traces and made power pours for microcontroller and display, also changed 4.7, 1uF and 2.2uF caps to 0402
</commit_message>
<xml_diff>
--- a/Passives_BOM.xlsx
+++ b/Passives_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ghani\Documents\ECE Projects\Variable_Voltage_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6282221B-D3CE-42FF-A46B-73B48D1F1F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4AC2B8-EBD7-4238-9FCA-9EA527ED70AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="-5790" windowWidth="14610" windowHeight="15585" firstSheet="2" activeTab="5" xr2:uid="{16F76EAB-28E7-44E5-8787-201DB1EE94CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16F76EAB-28E7-44E5-8787-201DB1EE94CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacitors" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Size</t>
   </si>
   <si>
-    <t>CL10B105KP8NNNC</t>
-  </si>
-  <si>
     <t>Tolerance %</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>C108, C109, C110, C112, C113, C115</t>
   </si>
   <si>
-    <t>CL10A225KO8NNNC</t>
-  </si>
-  <si>
     <t>Voltage Rating (V)</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t>CL10A475KP8NNNC</t>
-  </si>
-  <si>
     <t>C121</t>
   </si>
   <si>
@@ -413,6 +404,15 @@
   </si>
   <si>
     <t>J201</t>
+  </si>
+  <si>
+    <t>GRM155R60J475KE96D</t>
+  </si>
+  <si>
+    <t>CL05A105KP5NNNC</t>
+  </si>
+  <si>
+    <t>GRM155R61E225ME15D</t>
   </si>
 </sst>
 </file>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63176262-04E9-4B3B-A264-4D90E2BEFF9E}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,24 +829,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -855,18 +855,18 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -878,15 +878,15 @@
         <v>1206</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -895,18 +895,18 @@
         <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -915,38 +915,38 @@
         <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -955,18 +955,18 @@
         <v>50</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -975,18 +975,18 @@
         <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -995,18 +995,18 @@
         <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -1015,30 +1015,30 @@
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>6.3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1050,21 +1050,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://jlcpcb.com/partdetail/97047-CL10B105KP8NNNC/C95843" xr:uid="{7333A1B7-9249-4C10-A804-740B044AC54F}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://jlcpcb.com/partdetail/MurataElectronics-GRM31CR61E226KE15L/C77091" xr:uid="{30B79D20-E56B-411E-94F6-A51FC141EC87}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://jlcpcb.com/partdetail/166764-CL05B104KA5NNNC/C155422" xr:uid="{E8D08709-90FF-46F9-B047-6F32F15A6EFF}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://jlcpcb.com/partdetail/MurataElectronics-GRM21BR61E106KA73L/C84416" xr:uid="{29757E89-95B6-4F53-AE14-3E2CD08803D8}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://jlcpcb.com/partdetail/24366-CL10A225KO8NNNC/C23630" xr:uid="{D91DBDC6-905B-493F-BCC5-D47EF9BB54D5}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://jlcpcb.com/partdetail/Walsin_TechCorp-0402N140J500CT/C458857" xr:uid="{5AE468E6-5BF2-4141-8FE2-B7CD1FB6EE35}"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://jlcpcb.com/partdetail/196998-GRM1885C1H241JA01D/C185593" xr:uid="{0169278E-7FDB-4027-A196-747629C8826E}"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://jlcpcb.com/partdetail/Panasonic-EEEFTH101XAP/C165974" xr:uid="{7CE7F449-8C83-468A-9821-D0E9F9333579}"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://jlcpcb.com/partdetail/MurataElectronics-GRM155R71E103KA01D/C77013" xr:uid="{04D013D1-325A-496B-B862-909074D94D46}"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://jlcpcb.com/partdetail/2057-CL10A475KP8NNNC/C1705" xr:uid="{353B2E10-1DC0-4E26-9913-7624C208DB29}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://jlcpcb.com/partdetail/MurataElectronics-GRM31CR61E226KE15L/C77091" xr:uid="{30B79D20-E56B-411E-94F6-A51FC141EC87}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://jlcpcb.com/partdetail/166764-CL05B104KA5NNNC/C155422" xr:uid="{E8D08709-90FF-46F9-B047-6F32F15A6EFF}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://jlcpcb.com/partdetail/MurataElectronics-GRM21BR61E106KA73L/C84416" xr:uid="{29757E89-95B6-4F53-AE14-3E2CD08803D8}"/>
+    <hyperlink ref="B7" r:id="rId4" display="https://jlcpcb.com/partdetail/Walsin_TechCorp-0402N140J500CT/C458857" xr:uid="{5AE468E6-5BF2-4141-8FE2-B7CD1FB6EE35}"/>
+    <hyperlink ref="B8" r:id="rId5" display="https://jlcpcb.com/partdetail/196998-GRM1885C1H241JA01D/C185593" xr:uid="{0169278E-7FDB-4027-A196-747629C8826E}"/>
+    <hyperlink ref="B9" r:id="rId6" display="https://jlcpcb.com/partdetail/Panasonic-EEEFTH101XAP/C165974" xr:uid="{7CE7F449-8C83-468A-9821-D0E9F9333579}"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://jlcpcb.com/partdetail/MurataElectronics-GRM155R71E103KA01D/C77013" xr:uid="{04D013D1-325A-496B-B862-909074D94D46}"/>
+    <hyperlink ref="B11" r:id="rId8" display="https://jlcpcb.com/partdetail/MurataElectronics-GRM155R60J475KE96D/C76995" xr:uid="{473065AF-13E6-40FA-B4C9-7F531DF05520}"/>
+    <hyperlink ref="B2" r:id="rId9" display="https://jlcpcb.com/partdetail/15107-CL05A105KP5NNNC/C14445" xr:uid="{2FA5EBCF-0276-4CB9-B311-6F4DD83FA548}"/>
+    <hyperlink ref="B6" r:id="rId10" display="https://jlcpcb.com/partdetail/MurataElectronics-GRM155R61E225ME15D/C72203" xr:uid="{FD80D378-B101-4360-B099-D7CAFED95375}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="E2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1088,30 +1085,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4">
         <v>0.2</v>
@@ -1120,10 +1117,10 @@
         <v>7.2</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1150,262 +1147,262 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <v>0.1</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>0.1</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <v>0.5</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1453,42 +1450,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C2">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1520,18 +1517,18 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
         <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52525879-3B94-43C6-B780-A84620322222}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1561,102 +1558,102 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>102</v>
       </c>
-      <c r="C2" t="s">
-        <v>105</v>
-      </c>
       <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
         <v>106</v>
-      </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1">
         <v>1984617</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B4" s="1">
         <v>1984617</v>
       </c>
       <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
         <v>113</v>
-      </c>
-      <c r="D4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" t="s">
         <v>119</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>120</v>
-      </c>
-      <c r="D5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>